<commit_message>
first update with taskscheduleR
</commit_message>
<xml_diff>
--- a/data/s_labour.xlsx
+++ b/data/s_labour.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateocaicedo/Desktop/ITR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72a93ddaa5316df0/Dokumente/R-scripts/cepremap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951E9FA3-E693-3F46-98E6-82D56C57345A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{951E9FA3-E693-3F46-98E6-82D56C57345A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FACF058-7A94-4B43-8492-1B5C576FD298}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="s_labour" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="64">
   <si>
     <t>country</t>
   </si>
@@ -206,6 +211,24 @@
   </si>
   <si>
     <t>D995C_SPLIT</t>
+  </si>
+  <si>
+    <t>2018-01-01</t>
+  </si>
+  <si>
+    <t>2019-01-01</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
+  </si>
+  <si>
+    <t>2021-01-01</t>
+  </si>
+  <si>
+    <t>2022-01-01</t>
+  </si>
+  <si>
+    <t>2023-01-01</t>
   </si>
 </sst>
 </file>
@@ -426,7 +449,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -722,26 +745,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="1006" width="11.5"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="1006" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +807,7 @@
       <c r="N1" s="17"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -796,11 +819,11 @@
         <v>-905.39530848891297</v>
       </c>
       <c r="D2" s="17">
-        <f>-J2-K2-L2-M2</f>
+        <f t="shared" ref="D2:D24" si="0">-J2-K2-L2-M2</f>
         <v>-5762</v>
       </c>
       <c r="E2" s="2">
-        <f>H2+K2</f>
+        <f t="shared" ref="E2:E24" si="1">H2+K2</f>
         <v>516.85849887282393</v>
       </c>
       <c r="F2">
@@ -827,7 +850,7 @@
       <c r="N2" s="17"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -835,15 +858,15 @@
         <v>9</v>
       </c>
       <c r="C3" s="17">
-        <f t="shared" ref="C3:C24" si="0">F3+G3</f>
+        <f t="shared" ref="C3:C24" si="2">F3+G3</f>
         <v>-874.53774877409296</v>
       </c>
       <c r="D3" s="17">
-        <f>-J3-K3-L3-M3</f>
+        <f t="shared" si="0"/>
         <v>-5680</v>
       </c>
       <c r="E3" s="2">
-        <f>H3+K3</f>
+        <f t="shared" si="1"/>
         <v>564.06200860118702</v>
       </c>
       <c r="F3">
@@ -870,7 +893,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -878,15 +901,15 @@
         <v>10</v>
       </c>
       <c r="C4" s="17">
+        <f t="shared" si="2"/>
+        <v>-876.37787029748904</v>
+      </c>
+      <c r="D4" s="17">
         <f t="shared" si="0"/>
-        <v>-876.37787029748904</v>
-      </c>
-      <c r="D4" s="17">
-        <f>-J4-K4-L4-M4</f>
         <v>-6283</v>
       </c>
       <c r="E4" s="2">
-        <f>H4+K4</f>
+        <f t="shared" si="1"/>
         <v>639.14135115423892</v>
       </c>
       <c r="F4">
@@ -913,7 +936,7 @@
       <c r="N4" s="17"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -921,15 +944,15 @@
         <v>11</v>
       </c>
       <c r="C5" s="17">
+        <f t="shared" si="2"/>
+        <v>-909.74236269490905</v>
+      </c>
+      <c r="D5" s="17">
         <f t="shared" si="0"/>
-        <v>-909.74236269490905</v>
-      </c>
-      <c r="D5" s="17">
-        <f>-J5-K5-L5-M5</f>
         <v>-7157</v>
       </c>
       <c r="E5" s="2">
-        <f>H5+K5</f>
+        <f t="shared" si="1"/>
         <v>761.58452831912405</v>
       </c>
       <c r="F5">
@@ -956,7 +979,7 @@
       <c r="N5" s="17"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -964,15 +987,15 @@
         <v>12</v>
       </c>
       <c r="C6" s="17">
+        <f t="shared" si="2"/>
+        <v>-977.85989263875001</v>
+      </c>
+      <c r="D6" s="17">
         <f t="shared" si="0"/>
-        <v>-977.85989263875001</v>
-      </c>
-      <c r="D6" s="17">
-        <f>-J6-K6-L6-M6</f>
         <v>-7601</v>
       </c>
       <c r="E6" s="2">
-        <f>H6+K6</f>
+        <f t="shared" si="1"/>
         <v>734.49155738898901</v>
       </c>
       <c r="F6">
@@ -999,7 +1022,7 @@
       <c r="N6" s="17"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1007,15 +1030,15 @@
         <v>13</v>
       </c>
       <c r="C7" s="17">
+        <f t="shared" si="2"/>
+        <v>-1012.38071210982</v>
+      </c>
+      <c r="D7" s="17">
         <f t="shared" si="0"/>
-        <v>-1012.38071210982</v>
-      </c>
-      <c r="D7" s="17">
-        <f>-J7-K7-L7-M7</f>
         <v>-7904</v>
       </c>
       <c r="E7" s="2">
-        <f>H7+K7</f>
+        <f t="shared" si="1"/>
         <v>781.55120990475393</v>
       </c>
       <c r="F7">
@@ -1042,7 +1065,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1050,15 +1073,15 @@
         <v>14</v>
       </c>
       <c r="C8" s="17">
+        <f t="shared" si="2"/>
+        <v>-1056.27488558765</v>
+      </c>
+      <c r="D8" s="17">
         <f t="shared" si="0"/>
-        <v>-1056.27488558765</v>
-      </c>
-      <c r="D8" s="17">
-        <f>-J8-K8-L8-M8</f>
         <v>-8947</v>
       </c>
       <c r="E8" s="2">
-        <f>H8+K8</f>
+        <f t="shared" si="1"/>
         <v>787.81462023763106</v>
       </c>
       <c r="F8">
@@ -1085,7 +1108,7 @@
       <c r="N8" s="17"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1093,15 +1116,15 @@
         <v>15</v>
       </c>
       <c r="C9" s="17">
+        <f t="shared" si="2"/>
+        <v>-1070.37563170352</v>
+      </c>
+      <c r="D9" s="17">
         <f t="shared" si="0"/>
-        <v>-1070.37563170352</v>
-      </c>
-      <c r="D9" s="17">
-        <f>-J9-K9-L9-M9</f>
         <v>-8761</v>
       </c>
       <c r="E9" s="2">
-        <f>H9+K9</f>
+        <f t="shared" si="1"/>
         <v>787.83719640915206</v>
       </c>
       <c r="F9">
@@ -1128,7 +1151,7 @@
       <c r="N9" s="17"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1136,15 +1159,15 @@
         <v>16</v>
       </c>
       <c r="C10" s="17">
+        <f t="shared" si="2"/>
+        <v>-1112.5710465771399</v>
+      </c>
+      <c r="D10" s="17">
         <f t="shared" si="0"/>
-        <v>-1112.5710465771399</v>
-      </c>
-      <c r="D10" s="17">
-        <f>-J10-K10-L10-M10</f>
         <v>-9295</v>
       </c>
       <c r="E10" s="2">
-        <f>H10+K10</f>
+        <f t="shared" si="1"/>
         <v>844.94853424805797</v>
       </c>
       <c r="F10">
@@ -1171,7 +1194,7 @@
       <c r="N10" s="17"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1179,15 +1202,15 @@
         <v>17</v>
       </c>
       <c r="C11" s="17">
+        <f t="shared" si="2"/>
+        <v>-1154.75229563062</v>
+      </c>
+      <c r="D11" s="17">
         <f t="shared" si="0"/>
-        <v>-1154.75229563062</v>
-      </c>
-      <c r="D11" s="17">
-        <f>-J11-K11-L11-M11</f>
         <v>-10140</v>
       </c>
       <c r="E11" s="2">
-        <f>H11+K11</f>
+        <f t="shared" si="1"/>
         <v>866.67428258233303</v>
       </c>
       <c r="F11">
@@ -1214,7 +1237,7 @@
       <c r="N11" s="17"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1222,15 +1245,15 @@
         <v>18</v>
       </c>
       <c r="C12" s="17">
+        <f t="shared" si="2"/>
+        <v>-1266.6386619550301</v>
+      </c>
+      <c r="D12" s="17">
         <f t="shared" si="0"/>
-        <v>-1266.6386619550301</v>
-      </c>
-      <c r="D12" s="17">
-        <f>-J12-K12-L12-M12</f>
         <v>-9735</v>
       </c>
       <c r="E12" s="2">
-        <f>H12+K12</f>
+        <f t="shared" si="1"/>
         <v>842.51482613520602</v>
       </c>
       <c r="F12">
@@ -1257,7 +1280,7 @@
       <c r="N12" s="17"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1265,15 +1288,15 @@
         <v>19</v>
       </c>
       <c r="C13" s="17">
+        <f t="shared" si="2"/>
+        <v>-1266.51049450806</v>
+      </c>
+      <c r="D13" s="17">
         <f t="shared" si="0"/>
-        <v>-1266.51049450806</v>
-      </c>
-      <c r="D13" s="17">
-        <f>-J13-K13-L13-M13</f>
         <v>-5096</v>
       </c>
       <c r="E13" s="2">
-        <f>H13+K13</f>
+        <f t="shared" si="1"/>
         <v>865.32721736293399</v>
       </c>
       <c r="F13">
@@ -1300,7 +1323,7 @@
       <c r="N13" s="17"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1308,15 +1331,15 @@
         <v>20</v>
       </c>
       <c r="C14" s="17">
+        <f t="shared" si="2"/>
+        <v>-1605.9536422926601</v>
+      </c>
+      <c r="D14" s="17">
         <f t="shared" si="0"/>
-        <v>-1605.9536422926601</v>
-      </c>
-      <c r="D14" s="17">
-        <f>-J14-K14-L14-M14</f>
         <v>-5575</v>
       </c>
       <c r="E14" s="2">
-        <f>H14+K14</f>
+        <f t="shared" si="1"/>
         <v>790.64298766034403</v>
       </c>
       <c r="F14">
@@ -1343,7 +1366,7 @@
       <c r="N14" s="17"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1351,15 +1374,15 @@
         <v>21</v>
       </c>
       <c r="C15" s="17">
+        <f t="shared" si="2"/>
+        <v>-1680.6282142684699</v>
+      </c>
+      <c r="D15" s="17">
         <f t="shared" si="0"/>
-        <v>-1680.6282142684699</v>
-      </c>
-      <c r="D15" s="17">
-        <f>-J15-K15-L15-M15</f>
         <v>-6212</v>
       </c>
       <c r="E15" s="2">
-        <f>H15+K15</f>
+        <f t="shared" si="1"/>
         <v>816.54690982252805</v>
       </c>
       <c r="F15">
@@ -1386,7 +1409,7 @@
       <c r="N15" s="17"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1394,15 +1417,15 @@
         <v>22</v>
       </c>
       <c r="C16" s="17">
+        <f t="shared" si="2"/>
+        <v>-1664.9651716624301</v>
+      </c>
+      <c r="D16" s="17">
         <f t="shared" si="0"/>
-        <v>-1664.9651716624301</v>
-      </c>
-      <c r="D16" s="17">
-        <f>-J16-K16-L16-M16</f>
         <v>-6164</v>
       </c>
       <c r="E16" s="2">
-        <f>H16+K16</f>
+        <f t="shared" si="1"/>
         <v>850.67132720618997</v>
       </c>
       <c r="F16">
@@ -1429,7 +1452,7 @@
       <c r="N16" s="17"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1437,15 +1460,15 @@
         <v>23</v>
       </c>
       <c r="C17" s="17">
+        <f t="shared" si="2"/>
+        <v>5252.2902307554596</v>
+      </c>
+      <c r="D17" s="17">
         <f t="shared" si="0"/>
-        <v>5252.2902307554596</v>
-      </c>
-      <c r="D17" s="17">
-        <f>-J17-K17-L17-M17</f>
         <v>-6460</v>
       </c>
       <c r="E17" s="2">
-        <f>H17+K17</f>
+        <f t="shared" si="1"/>
         <v>864.71626638501107</v>
       </c>
       <c r="F17">
@@ -1472,7 +1495,7 @@
       <c r="N17" s="17"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1480,15 +1503,15 @@
         <v>24</v>
       </c>
       <c r="C18" s="17">
+        <f t="shared" si="2"/>
+        <v>6089.9739119057394</v>
+      </c>
+      <c r="D18" s="17">
         <f t="shared" si="0"/>
-        <v>6089.9739119057394</v>
-      </c>
-      <c r="D18" s="17">
-        <f>-J18-K18-L18-M18</f>
         <v>-7557</v>
       </c>
       <c r="E18" s="2">
-        <f>H18+K18</f>
+        <f t="shared" si="1"/>
         <v>865.41657660379292</v>
       </c>
       <c r="F18">
@@ -1515,7 +1538,7 @@
       <c r="N18" s="17"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1523,15 +1546,15 @@
         <v>25</v>
       </c>
       <c r="C19" s="17">
+        <f t="shared" si="2"/>
+        <v>6605.9302509399604</v>
+      </c>
+      <c r="D19" s="17">
         <f t="shared" si="0"/>
-        <v>6605.9302509399604</v>
-      </c>
-      <c r="D19" s="17">
-        <f>-J19-K19-L19-M19</f>
         <v>-10360</v>
       </c>
       <c r="E19" s="2">
-        <f>H19+K19</f>
+        <f t="shared" si="1"/>
         <v>833.42361316327901</v>
       </c>
       <c r="F19">
@@ -1558,7 +1581,7 @@
       <c r="N19" s="17"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1566,15 +1589,15 @@
         <v>26</v>
       </c>
       <c r="C20" s="17">
+        <f t="shared" si="2"/>
+        <v>6250.2293886984799</v>
+      </c>
+      <c r="D20" s="17">
         <f t="shared" si="0"/>
-        <v>6250.2293886984799</v>
-      </c>
-      <c r="D20" s="17">
-        <f>-J20-K20-L20-M20</f>
         <v>-10433</v>
       </c>
       <c r="E20" s="2">
-        <f>H20+K20</f>
+        <f t="shared" si="1"/>
         <v>777.14863842438501</v>
       </c>
       <c r="F20">
@@ -1601,7 +1624,7 @@
       <c r="N20" s="17"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1609,15 +1632,15 @@
         <v>27</v>
       </c>
       <c r="C21" s="17">
+        <f t="shared" si="2"/>
+        <v>6668.3416625821201</v>
+      </c>
+      <c r="D21" s="17">
         <f t="shared" si="0"/>
-        <v>6668.3416625821201</v>
-      </c>
-      <c r="D21" s="17">
-        <f>-J21-K21-L21-M21</f>
         <v>-10216</v>
       </c>
       <c r="E21" s="2">
-        <f>H21+K21</f>
+        <f t="shared" si="1"/>
         <v>779.39068684336496</v>
       </c>
       <c r="F21">
@@ -1644,7 +1667,7 @@
       <c r="N21" s="17"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1652,15 +1675,15 @@
         <v>28</v>
       </c>
       <c r="C22" s="17">
+        <f t="shared" si="2"/>
+        <v>6703.55282788553</v>
+      </c>
+      <c r="D22" s="17">
         <f t="shared" si="0"/>
-        <v>6703.55282788553</v>
-      </c>
-      <c r="D22" s="17">
-        <f>-J22-K22-L22-M22</f>
         <v>-10519</v>
       </c>
       <c r="E22" s="2">
-        <f>H22+K22</f>
+        <f t="shared" si="1"/>
         <v>590.36310617363097</v>
       </c>
       <c r="F22">
@@ -1687,7 +1710,7 @@
       <c r="N22" s="17"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1695,15 +1718,15 @@
         <v>29</v>
       </c>
       <c r="C23" s="17">
+        <f t="shared" si="2"/>
+        <v>7142.4248927399603</v>
+      </c>
+      <c r="D23" s="17">
         <f t="shared" si="0"/>
-        <v>7142.4248927399603</v>
-      </c>
-      <c r="D23" s="17">
-        <f>-J23-K23-L23-M23</f>
         <v>-10738</v>
       </c>
       <c r="E23" s="2">
-        <f>H23+K23</f>
+        <f t="shared" si="1"/>
         <v>601.98560365137405</v>
       </c>
       <c r="F23">
@@ -1730,7 +1753,7 @@
       <c r="N23" s="17"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1738,15 +1761,15 @@
         <v>30</v>
       </c>
       <c r="C24" s="17">
+        <f t="shared" si="2"/>
+        <v>7156.22787905716</v>
+      </c>
+      <c r="D24" s="17">
         <f t="shared" si="0"/>
-        <v>7156.22787905716</v>
-      </c>
-      <c r="D24" s="17">
-        <f>-J24-K24-L24-M24</f>
         <v>-11293</v>
       </c>
       <c r="E24" s="2">
-        <f>H24+K24</f>
+        <f t="shared" si="1"/>
         <v>871.24612547017898</v>
       </c>
       <c r="F24">
@@ -1773,575 +1796,713 @@
       <c r="N24" s="17"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="C25" s="17"/>
-      <c r="D25" s="17">
-        <f>I25</f>
-        <v>-941.45258279379561</v>
-      </c>
-      <c r="E25" s="17"/>
-      <c r="I25" s="17">
-        <v>-941.45258279379561</v>
-      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="2"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
       <c r="K25" s="17"/>
       <c r="L25" s="17"/>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="C26" s="17"/>
-      <c r="D26" s="17">
-        <f t="shared" ref="D26:D47" si="1">I26</f>
-        <v>-772.11903039073809</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="I26" s="17">
-        <v>-772.11903039073809</v>
-      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="2"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C27" s="17"/>
-      <c r="D27" s="17">
-        <f t="shared" si="1"/>
-        <v>-856.95470911886071</v>
-      </c>
-      <c r="E27" s="17"/>
-      <c r="I27" s="17">
-        <v>-856.95470911886071</v>
-      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="2"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="C28" s="17"/>
-      <c r="D28" s="17">
-        <f t="shared" si="1"/>
-        <v>-768.86053991958636</v>
-      </c>
-      <c r="E28" s="17"/>
-      <c r="I28" s="17">
-        <v>-768.86053991958636</v>
-      </c>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="2"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="C29" s="17"/>
-      <c r="D29" s="17">
-        <f t="shared" si="1"/>
-        <v>-820.61182671895801</v>
-      </c>
-      <c r="E29" s="17"/>
-      <c r="I29" s="17">
-        <v>-820.61182671895801</v>
-      </c>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="2"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C30" s="17"/>
-      <c r="D30" s="17">
-        <f t="shared" si="1"/>
-        <v>-843.53793974323685</v>
-      </c>
-      <c r="E30" s="17"/>
-      <c r="I30" s="17">
-        <v>-843.53793974323685</v>
-      </c>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="2"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17">
-        <f t="shared" si="1"/>
-        <v>-843.71550100261288</v>
+        <f>I31</f>
+        <v>-941.45258279379561</v>
       </c>
       <c r="E31" s="17"/>
       <c r="I31" s="17">
-        <v>-843.71550100261288</v>
-      </c>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+        <v>-941.45258279379561</v>
+      </c>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17">
-        <f t="shared" si="1"/>
-        <v>-926.41050010096239</v>
+        <f t="shared" ref="D32:D53" si="3">I32</f>
+        <v>-772.11903039073809</v>
       </c>
       <c r="E32" s="17"/>
       <c r="I32" s="17">
-        <v>-926.41050010096239</v>
-      </c>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+        <v>-772.11903039073809</v>
+      </c>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17">
-        <f t="shared" si="1"/>
-        <v>-854.80816929653292</v>
+        <f t="shared" si="3"/>
+        <v>-856.95470911886071</v>
       </c>
       <c r="E33" s="17"/>
       <c r="I33" s="17">
-        <v>-854.80816929653292</v>
-      </c>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+        <v>-856.95470911886071</v>
+      </c>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17">
-        <f t="shared" si="1"/>
-        <v>-876.68243990865653</v>
+        <f t="shared" si="3"/>
+        <v>-768.86053991958636</v>
       </c>
       <c r="E34" s="17"/>
       <c r="I34" s="17">
-        <v>-876.68243990865653</v>
+        <v>-768.86053991958636</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17">
-        <f t="shared" si="1"/>
-        <v>-911.62424503882653</v>
+        <f t="shared" si="3"/>
+        <v>-820.61182671895801</v>
       </c>
       <c r="E35" s="17"/>
       <c r="I35" s="17">
-        <v>-911.62424503882653</v>
+        <v>-820.61182671895801</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="17">
-        <f t="shared" si="1"/>
-        <v>-1242.431014187473</v>
+        <f t="shared" si="3"/>
+        <v>-843.53793974323685</v>
       </c>
       <c r="E36" s="17"/>
       <c r="I36" s="17">
-        <v>-1242.431014187473</v>
+        <v>-843.53793974323685</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17">
-        <f t="shared" si="1"/>
-        <v>-1408.6016143175125</v>
+        <f t="shared" si="3"/>
+        <v>-843.71550100261288</v>
       </c>
       <c r="E37" s="17"/>
       <c r="I37" s="17">
-        <v>-1408.6016143175125</v>
+        <v>-843.71550100261288</v>
       </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>31</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17">
-        <f t="shared" si="1"/>
-        <v>-1607.1301279815405</v>
+        <f t="shared" si="3"/>
+        <v>-926.41050010096239</v>
       </c>
       <c r="E38" s="17"/>
       <c r="I38" s="17">
-        <v>-1607.1301279815405</v>
+        <v>-926.41050010096239</v>
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>31</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C39" s="17"/>
       <c r="D39" s="17">
-        <f t="shared" si="1"/>
-        <v>-2531.5137748972816</v>
+        <f t="shared" si="3"/>
+        <v>-854.80816929653292</v>
       </c>
       <c r="E39" s="17"/>
       <c r="I39" s="17">
-        <v>-2531.5137748972816</v>
+        <v>-854.80816929653292</v>
       </c>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C40" s="17"/>
       <c r="D40" s="17">
-        <f t="shared" si="1"/>
-        <v>-2639.1609063999181</v>
+        <f t="shared" si="3"/>
+        <v>-876.68243990865653</v>
       </c>
       <c r="E40" s="17"/>
       <c r="I40" s="17">
-        <v>-2639.1609063999181</v>
+        <v>-876.68243990865653</v>
       </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>31</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="17">
-        <f t="shared" si="1"/>
-        <v>-2718.9928492295298</v>
+        <f t="shared" si="3"/>
+        <v>-911.62424503882653</v>
       </c>
       <c r="E41" s="17"/>
       <c r="I41" s="17">
-        <v>-2718.9928492295298</v>
+        <v>-911.62424503882653</v>
       </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>31</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C42" s="17"/>
       <c r="D42" s="17">
-        <f t="shared" si="1"/>
-        <v>-2199.3114005248322</v>
+        <f t="shared" si="3"/>
+        <v>-1242.431014187473</v>
       </c>
       <c r="E42" s="17"/>
       <c r="I42" s="17">
-        <v>-2199.3114005248322</v>
+        <v>-1242.431014187473</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>31</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17">
-        <f t="shared" si="1"/>
-        <v>-2197.5992295351466</v>
+        <f t="shared" si="3"/>
+        <v>-1408.6016143175125</v>
       </c>
       <c r="E43" s="17"/>
       <c r="I43" s="17">
-        <v>-2197.5992295351466</v>
+        <v>-1408.6016143175125</v>
       </c>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>31</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="17">
-        <f t="shared" si="1"/>
-        <v>-1338.0454429209371</v>
+        <f t="shared" si="3"/>
+        <v>-1607.1301279815405</v>
       </c>
       <c r="E44" s="17"/>
       <c r="I44" s="17">
-        <v>-1338.0454429209371</v>
+        <v>-1607.1301279815405</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>31</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C45" s="17"/>
       <c r="D45" s="17">
-        <f t="shared" si="1"/>
-        <v>-2004.9438984983842</v>
+        <f t="shared" si="3"/>
+        <v>-2531.5137748972816</v>
       </c>
       <c r="E45" s="17"/>
       <c r="I45" s="17">
-        <v>-2004.9438984983842</v>
+        <v>-2531.5137748972816</v>
       </c>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C46" s="17"/>
       <c r="D46" s="17">
-        <f t="shared" si="1"/>
-        <v>-1485.5454869247353</v>
+        <f t="shared" si="3"/>
+        <v>-2639.1609063999181</v>
       </c>
       <c r="E46" s="17"/>
       <c r="I46" s="17">
-        <v>-1485.5454869247353</v>
+        <v>-2639.1609063999181</v>
       </c>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>31</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C47" s="17"/>
       <c r="D47" s="17">
-        <f t="shared" si="1"/>
-        <v>-1380.7409708669893</v>
+        <f t="shared" si="3"/>
+        <v>-2718.9928492295298</v>
       </c>
       <c r="E47" s="17"/>
       <c r="I47" s="17">
-        <v>-1380.7409708669893</v>
-      </c>
+        <v>-2718.9928492295298</v>
+      </c>
+      <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B48" s="1"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17">
+        <f t="shared" si="3"/>
+        <v>-2199.3114005248322</v>
+      </c>
+      <c r="E48" s="17"/>
+      <c r="I48" s="17">
+        <v>-2199.3114005248322</v>
+      </c>
+      <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B49" s="1"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17">
+        <f t="shared" si="3"/>
+        <v>-2197.5992295351466</v>
+      </c>
+      <c r="E49" s="17"/>
+      <c r="I49" s="17">
+        <v>-2197.5992295351466</v>
+      </c>
+      <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B50" s="1"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17">
+        <f t="shared" si="3"/>
+        <v>-1338.0454429209371</v>
+      </c>
+      <c r="E50" s="17"/>
+      <c r="I50" s="17">
+        <v>-1338.0454429209371</v>
+      </c>
+      <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B51" s="1"/>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17">
+        <f t="shared" si="3"/>
+        <v>-2004.9438984983842</v>
+      </c>
+      <c r="E51" s="17"/>
+      <c r="I51" s="17">
+        <v>-2004.9438984983842</v>
+      </c>
+      <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B52" s="1"/>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17">
+        <f t="shared" si="3"/>
+        <v>-1485.5454869247353</v>
+      </c>
+      <c r="E52" s="17"/>
+      <c r="I52" s="17">
+        <v>-1485.5454869247353</v>
+      </c>
+      <c r="L52" s="2"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B53" s="1"/>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17">
+        <f t="shared" si="3"/>
+        <v>-1380.7409708669893</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="I53" s="17">
+        <v>-1380.7409708669893</v>
+      </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B54" s="1"/>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
     </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B55" s="1"/>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
     </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B56" s="1"/>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.15">
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.15">
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B62" s="1"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="2"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2362,9 +2523,9 @@
       <selection activeCell="C1" sqref="C1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -2460,7 +2621,7 @@
         <v>203017</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
@@ -2556,7 +2717,7 @@
         <v>172283</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
@@ -2652,7 +2813,7 @@
         <v>11955</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>32</v>
       </c>
@@ -2748,7 +2909,7 @@
         <v>4766</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
@@ -2844,7 +3005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>47</v>
       </c>

</xml_diff>